<commit_message>
removed unnecessary shts in dashboard
</commit_message>
<xml_diff>
--- a/ProgramSrc/commData.xlsx
+++ b/ProgramSrc/commData.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,1108 +436,1388 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Active</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>Name</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>xDegrees</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>yDegrees</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Population</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>AffectedPop</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>WorkPop</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>MaxDistance</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Remarks</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" t="b">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
         <is>
           <t>Balite</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>14.8956</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>120.7855</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>5016</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
         <is>
           <t>2144</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" t="b">
+        <v>0</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
         <is>
           <t>Balungao</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>14.9143</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>120.7622</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>5720</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
         <is>
           <t>3366</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr"/>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" t="b">
+        <v>0</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
         <is>
           <t>Buguion</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>14.894</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="E4" t="inlineStr">
         <is>
           <t>120.7985</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="F4" t="inlineStr">
         <is>
           <t>3841</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
         <is>
           <t>2196</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr"/>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" t="b">
+        <v>1</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
         <is>
           <t>Bulusan</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t>14.9076</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t>120.7455</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t>2603</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
         <is>
           <t>1721</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="A6" t="b">
+        <v>0</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
         <is>
           <t>Calizon</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="D6" t="inlineStr">
         <is>
           <t>14.9125</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="E6" t="inlineStr">
         <is>
           <t>120.753</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="F6" t="inlineStr">
         <is>
           <t>2221</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
         <is>
           <t>1387</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr"/>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="A7" t="b">
+        <v>0</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
         <is>
           <t>Calumpang</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="D7" t="inlineStr">
         <is>
           <t>14.8845</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="E7" t="inlineStr">
         <is>
           <t>120.7838</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="F7" t="inlineStr">
         <is>
           <t>3517</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
         <is>
           <t>2784</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr"/>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
+      <c r="A8" t="b">
+        <v>0</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
         <is>
           <t>Caniogan</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="D8" t="inlineStr">
         <is>
           <t>14.9054</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="E8" t="inlineStr">
         <is>
           <t>120.7733</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="F8" t="inlineStr">
         <is>
           <t>4510</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
         <is>
           <t>2869</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr"/>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
+      <c r="A9" t="b">
+        <v>0</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
         <is>
           <t>Corazon</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="D9" t="inlineStr">
         <is>
           <t>14.9128</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="E9" t="inlineStr">
         <is>
           <t>120.7686</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="F9" t="inlineStr">
         <is>
           <t>2175</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
         <is>
           <t>1647</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr"/>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
+      <c r="A10" t="b">
+        <v>0</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
         <is>
           <t>Frances</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="D10" t="inlineStr">
         <is>
           <t>14.9153</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="E10" t="inlineStr">
         <is>
           <t>120.7532</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="F10" t="inlineStr">
         <is>
           <t>6129</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="G10" t="inlineStr">
         <is>
           <t>6</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
+      <c r="H10" t="inlineStr">
         <is>
           <t>3819</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr"/>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
+      <c r="A11" t="b">
+        <v>0</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
         <is>
           <t>Gatbuca</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="D11" t="inlineStr">
         <is>
           <t>14.9218</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="E11" t="inlineStr">
         <is>
           <t>120.7685</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="F11" t="inlineStr">
         <is>
           <t>6384</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
+      <c r="G11" t="inlineStr">
         <is>
           <t>115</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr">
+      <c r="H11" t="inlineStr">
         <is>
           <t>4250</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr"/>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
+      <c r="A12" t="b">
+        <v>0</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
         <is>
           <t>Gugo</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="D12" t="inlineStr">
         <is>
           <t>14.9014</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="E12" t="inlineStr">
         <is>
           <t>120.7548</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="F12" t="inlineStr">
         <is>
           <t>1960</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr">
+      <c r="G12" t="inlineStr">
         <is>
           <t>57</t>
         </is>
       </c>
-      <c r="F12" t="inlineStr">
+      <c r="H12" t="inlineStr">
         <is>
           <t>1179</t>
         </is>
       </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr"/>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
+      <c r="A13" t="b">
+        <v>0</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
         <is>
           <t>Iba Este</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="D13" t="inlineStr">
         <is>
           <t>14.8899</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="E13" t="inlineStr">
         <is>
           <t>120.7673</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
+      <c r="F13" t="inlineStr">
         <is>
           <t>4161</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
         <is>
           <t>1828</t>
         </is>
       </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr"/>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
+      <c r="A14" t="b">
+        <v>0</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
         <is>
           <t>Iba O'Este</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
+      <c r="D14" t="inlineStr">
         <is>
           <t>14.8919</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
+      <c r="E14" t="inlineStr">
         <is>
           <t>120.7635</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
+      <c r="F14" t="inlineStr">
         <is>
           <t>14085</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr">
+      <c r="G14" t="inlineStr">
         <is>
           <t>601</t>
         </is>
       </c>
-      <c r="F14" t="inlineStr">
+      <c r="H14" t="inlineStr">
         <is>
           <t>8095</t>
         </is>
       </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr"/>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
+      <c r="A15" t="b">
+        <v>0</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
         <is>
           <t>Longos</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
+      <c r="D15" t="inlineStr">
         <is>
           <t>14.8748</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="E15" t="inlineStr">
         <is>
           <t>120.7866</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
+      <c r="F15" t="inlineStr">
         <is>
           <t>4265</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
         <is>
           <t>2293</t>
         </is>
       </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr"/>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr"/>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
+      <c r="A16" t="b">
+        <v>0</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
         <is>
           <t>Meysulao</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
+      <c r="D16" t="inlineStr">
         <is>
           <t>14.9078</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
+      <c r="E16" t="inlineStr">
         <is>
           <t>120.7397</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
+      <c r="F16" t="inlineStr">
         <is>
           <t>4280</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr">
+      <c r="G16" t="inlineStr">
         <is>
           <t>56</t>
         </is>
       </c>
-      <c r="F16" t="inlineStr">
+      <c r="H16" t="inlineStr">
         <is>
           <t>2687</t>
         </is>
       </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr"/>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr"/>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr">
+      <c r="A17" t="b">
+        <v>0</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
         <is>
           <t>Meyto</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
+      <c r="D17" t="inlineStr">
         <is>
           <t>14.8831</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
+      <c r="E17" t="inlineStr">
         <is>
           <t>120.7295</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr">
+      <c r="F17" t="inlineStr">
         <is>
           <t>2925</t>
         </is>
       </c>
-      <c r="E17" t="inlineStr">
+      <c r="G17" t="inlineStr">
         <is>
           <t>6</t>
         </is>
       </c>
-      <c r="F17" t="inlineStr">
+      <c r="H17" t="inlineStr">
         <is>
           <t>1975</t>
         </is>
       </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr"/>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr"/>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
+      <c r="A18" t="b">
+        <v>0</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
         <is>
           <t>Palimbang</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
+      <c r="D18" t="inlineStr">
         <is>
           <t>14.8994</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
+      <c r="E18" t="inlineStr">
         <is>
           <t>120.7756</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr">
+      <c r="F18" t="inlineStr">
         <is>
           <t>1684</t>
         </is>
       </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
         <is>
           <t>1424</t>
         </is>
       </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="H18" t="inlineStr"/>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr"/>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr">
+      <c r="A19" t="b">
+        <v>0</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
         <is>
           <t>Panducot</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr">
+      <c r="D19" t="inlineStr">
         <is>
           <t>14.8761</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr">
+      <c r="E19" t="inlineStr">
         <is>
           <t>120.738</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr">
+      <c r="F19" t="inlineStr">
         <is>
           <t>1752</t>
         </is>
       </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
         <is>
           <t>1713</t>
         </is>
       </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="H19" t="inlineStr"/>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr"/>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr">
+      <c r="A20" t="b">
+        <v>0</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
         <is>
           <t>Poblacion</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr">
+      <c r="D20" t="inlineStr">
         <is>
           <t>14.9157</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr">
+      <c r="E20" t="inlineStr">
         <is>
           <t>120.7672</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr">
+      <c r="F20" t="inlineStr">
         <is>
           <t>1785</t>
         </is>
       </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
         <is>
           <t>1294</t>
         </is>
       </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr"/>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr"/>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr">
+      <c r="A21" t="b">
+        <v>0</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
         <is>
           <t>Pungo</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr">
+      <c r="D21" t="inlineStr">
         <is>
           <t>14.9023</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
+      <c r="E21" t="inlineStr">
         <is>
           <t>120.7914</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr">
+      <c r="F21" t="inlineStr">
         <is>
           <t>9528</t>
         </is>
       </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
         <is>
           <t>5486</t>
         </is>
       </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="H21" t="inlineStr"/>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr"/>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr">
+      <c r="A22" t="b">
+        <v>0</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
         <is>
           <t>San Jose</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr">
+      <c r="D22" t="inlineStr">
         <is>
           <t>14.8838</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr">
+      <c r="E22" t="inlineStr">
         <is>
           <t>120.7395</t>
         </is>
       </c>
-      <c r="D22" t="inlineStr">
+      <c r="F22" t="inlineStr">
         <is>
           <t>5661</t>
         </is>
       </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
         <is>
           <t>3629</t>
         </is>
       </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="H22" t="inlineStr"/>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr"/>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr">
+      <c r="A23" t="b">
+        <v>0</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
         <is>
           <t>San Marcos</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr">
+      <c r="D23" t="inlineStr">
         <is>
           <t>14.8976</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr">
+      <c r="E23" t="inlineStr">
         <is>
           <t>120.7797</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr">
+      <c r="F23" t="inlineStr">
         <is>
           <t>2671</t>
         </is>
       </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr">
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
         <is>
           <t>1471</t>
         </is>
       </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="H23" t="inlineStr"/>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr"/>
     </row>
     <row r="24">
-      <c r="A24" t="inlineStr">
+      <c r="A24" t="b">
+        <v>0</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
         <is>
           <t>San Miguel</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr">
+      <c r="D24" t="inlineStr">
         <is>
           <t>14.917</t>
         </is>
       </c>
-      <c r="C24" t="inlineStr">
+      <c r="E24" t="inlineStr">
         <is>
           <t>120.7427</t>
         </is>
       </c>
-      <c r="D24" t="inlineStr">
+      <c r="F24" t="inlineStr">
         <is>
           <t>6005</t>
         </is>
       </c>
-      <c r="E24" t="inlineStr">
+      <c r="G24" t="inlineStr">
         <is>
           <t>17</t>
         </is>
       </c>
-      <c r="F24" t="inlineStr">
+      <c r="H24" t="inlineStr">
         <is>
           <t>3287</t>
         </is>
       </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="H24" t="inlineStr"/>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr"/>
     </row>
     <row r="25">
-      <c r="A25" t="inlineStr">
+      <c r="A25" t="b">
+        <v>0</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
         <is>
           <t>Santa Lucia</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr">
+      <c r="D25" t="inlineStr">
         <is>
           <t>14.8982</t>
         </is>
       </c>
-      <c r="C25" t="inlineStr">
+      <c r="E25" t="inlineStr">
         <is>
           <t>120.736</t>
         </is>
       </c>
-      <c r="D25" t="inlineStr">
+      <c r="F25" t="inlineStr">
         <is>
           <t>2460</t>
         </is>
       </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F25" t="inlineStr">
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
         <is>
           <t>1483</t>
         </is>
       </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="H25" t="inlineStr"/>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr"/>
     </row>
     <row r="26">
-      <c r="A26" t="inlineStr">
+      <c r="A26" t="b">
+        <v>0</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
         <is>
           <t>Santo Niño</t>
         </is>
       </c>
-      <c r="B26" t="inlineStr">
+      <c r="D26" t="inlineStr">
         <is>
           <t>14.9047</t>
         </is>
       </c>
-      <c r="C26" t="inlineStr">
+      <c r="E26" t="inlineStr">
         <is>
           <t>120.7792</t>
         </is>
       </c>
-      <c r="D26" t="inlineStr">
+      <c r="F26" t="inlineStr">
         <is>
           <t>2544</t>
         </is>
       </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F26" t="inlineStr">
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
         <is>
           <t>1392</t>
         </is>
       </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="H26" t="inlineStr"/>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr"/>
     </row>
     <row r="27">
-      <c r="A27" t="inlineStr">
+      <c r="A27" t="b">
+        <v>0</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
         <is>
           <t>Sapang Bayan</t>
         </is>
       </c>
-      <c r="B27" t="inlineStr">
+      <c r="D27" t="inlineStr">
         <is>
           <t>14.9196</t>
         </is>
       </c>
-      <c r="C27" t="inlineStr">
+      <c r="E27" t="inlineStr">
         <is>
           <t>120.7739</t>
         </is>
       </c>
-      <c r="D27" t="inlineStr">
+      <c r="F27" t="inlineStr">
         <is>
           <t>3140</t>
         </is>
       </c>
-      <c r="E27" t="inlineStr">
+      <c r="G27" t="inlineStr">
         <is>
           <t>65</t>
         </is>
       </c>
-      <c r="F27" t="inlineStr">
+      <c r="H27" t="inlineStr">
         <is>
           <t>1775</t>
         </is>
       </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="H27" t="inlineStr"/>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr"/>
     </row>
     <row r="28">
-      <c r="A28" t="inlineStr">
+      <c r="A28" t="b">
+        <v>0</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
         <is>
           <t>Sergio Bayan</t>
         </is>
       </c>
-      <c r="B28" t="inlineStr">
+      <c r="D28" t="inlineStr">
         <is>
           <t>14.894</t>
         </is>
       </c>
-      <c r="C28" t="inlineStr">
+      <c r="E28" t="inlineStr">
         <is>
           <t>120.7909</t>
         </is>
       </c>
-      <c r="D28" t="inlineStr">
+      <c r="F28" t="inlineStr">
         <is>
           <t>1727</t>
         </is>
       </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F28" t="inlineStr">
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
         <is>
           <t>1258</t>
         </is>
       </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="H28" t="inlineStr"/>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr"/>
     </row>
     <row r="29">
-      <c r="A29" t="inlineStr">
+      <c r="A29" t="b">
+        <v>0</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
         <is>
           <t>Sucol</t>
         </is>
       </c>
-      <c r="B29" t="inlineStr">
+      <c r="D29" t="inlineStr">
         <is>
           <t>14.9138</t>
         </is>
       </c>
-      <c r="C29" t="inlineStr">
+      <c r="E29" t="inlineStr">
         <is>
           <t>120.7701</t>
         </is>
       </c>
-      <c r="D29" t="inlineStr">
+      <c r="F29" t="inlineStr">
         <is>
           <t>1059</t>
         </is>
       </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F29" t="inlineStr">
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
         <is>
           <t>963</t>
         </is>
       </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="H29" t="inlineStr"/>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr"/>
+    </row>
+    <row r="30">
+      <c r="A30" t="b">
+        <v>0</v>
+      </c>
+      <c r="B30" t="inlineStr"/>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>testAdd</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>120.0</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>12.0</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>32.0</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
updated switches more user-friendly
</commit_message>
<xml_diff>
--- a/ProgramSrc/commData.xlsx
+++ b/ProgramSrc/commData.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J30"/>
+  <dimension ref="A1:L30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,40 +446,50 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>Active.2</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Active.1</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>Name</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>xDegrees</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>yDegrees</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Population</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>AffectedPop</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>WorkPop</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>MaxDistance</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Remarks</t>
         </is>
@@ -491,183 +501,223 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>True</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
           <t>Balite</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>14.8956</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>120.7855</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>5016</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="I2" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="J2" t="inlineStr">
         <is>
           <t>2144</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>False</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
           <t>Balungao</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>14.9143</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="G3" t="inlineStr">
         <is>
           <t>120.7622</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="H3" t="inlineStr">
         <is>
           <t>5720</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="I3" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="J3" t="inlineStr">
         <is>
           <t>3366</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>False</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
           <t>Buguion</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="F4" t="inlineStr">
         <is>
           <t>14.894</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="G4" t="inlineStr">
         <is>
           <t>120.7985</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="H4" t="inlineStr">
         <is>
           <t>3841</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="I4" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
+      <c r="J4" t="inlineStr">
         <is>
           <t>2196</t>
         </is>
       </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
           <t>1.0</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t>Bulusan</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t>14.9076</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="G5" t="inlineStr">
         <is>
           <t>120.7455</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="H5" t="inlineStr">
         <is>
           <t>2603</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
+      <c r="I5" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
+      <c r="J5" t="inlineStr">
         <is>
           <t>1721</t>
         </is>
       </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="b">
@@ -675,45 +725,55 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>False</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
           <t>Calizon</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="F6" t="inlineStr">
         <is>
           <t>14.9125</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="G6" t="inlineStr">
         <is>
           <t>120.753</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="H6" t="inlineStr">
         <is>
           <t>2221</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr">
+      <c r="I6" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr">
+      <c r="J6" t="inlineStr">
         <is>
           <t>1387</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="b">
@@ -721,183 +781,223 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>False</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
           <t>Calumpang</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="F7" t="inlineStr">
         <is>
           <t>14.8845</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="G7" t="inlineStr">
         <is>
           <t>120.7838</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="H7" t="inlineStr">
         <is>
           <t>3517</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
+      <c r="I7" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
+      <c r="J7" t="inlineStr">
         <is>
           <t>2784</t>
         </is>
       </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>False</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
           <t>Caniogan</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="F8" t="inlineStr">
         <is>
           <t>14.9054</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="G8" t="inlineStr">
         <is>
           <t>120.7733</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="H8" t="inlineStr">
         <is>
           <t>4510</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr">
+      <c r="I8" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr">
+      <c r="J8" t="inlineStr">
         <is>
           <t>2869</t>
         </is>
       </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>False</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
           <t>Corazon</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="F9" t="inlineStr">
         <is>
           <t>14.9128</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="G9" t="inlineStr">
         <is>
           <t>120.7686</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
+      <c r="H9" t="inlineStr">
         <is>
           <t>2175</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr">
+      <c r="I9" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="H9" t="inlineStr">
+      <c r="J9" t="inlineStr">
         <is>
           <t>1647</t>
         </is>
       </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>True</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
           <t>Frances</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="F10" t="inlineStr">
         <is>
           <t>14.9153</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="G10" t="inlineStr">
         <is>
           <t>120.7532</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
+      <c r="H10" t="inlineStr">
         <is>
           <t>6129</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr">
+      <c r="I10" t="inlineStr">
         <is>
           <t>6</t>
         </is>
       </c>
-      <c r="H10" t="inlineStr">
+      <c r="J10" t="inlineStr">
         <is>
           <t>3819</t>
         </is>
       </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="b">
@@ -905,45 +1005,55 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>False</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
           <t>Gatbuca</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="F11" t="inlineStr">
         <is>
           <t>14.9218</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
+      <c r="G11" t="inlineStr">
         <is>
           <t>120.7685</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr">
+      <c r="H11" t="inlineStr">
         <is>
           <t>6384</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr">
+      <c r="I11" t="inlineStr">
         <is>
           <t>115</t>
         </is>
       </c>
-      <c r="H11" t="inlineStr">
+      <c r="J11" t="inlineStr">
         <is>
           <t>4250</t>
         </is>
       </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="b">
@@ -951,45 +1061,55 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>False</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
           <t>Gugo</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="F12" t="inlineStr">
         <is>
           <t>14.9014</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr">
+      <c r="G12" t="inlineStr">
         <is>
           <t>120.7548</t>
         </is>
       </c>
-      <c r="F12" t="inlineStr">
+      <c r="H12" t="inlineStr">
         <is>
           <t>1960</t>
         </is>
       </c>
-      <c r="G12" t="inlineStr">
+      <c r="I12" t="inlineStr">
         <is>
           <t>57</t>
         </is>
       </c>
-      <c r="H12" t="inlineStr">
+      <c r="J12" t="inlineStr">
         <is>
           <t>1179</t>
         </is>
       </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="b">
@@ -997,45 +1117,55 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>False</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
           <t>Iba Este</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
+      <c r="F13" t="inlineStr">
         <is>
           <t>14.8899</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
+      <c r="G13" t="inlineStr">
         <is>
           <t>120.7673</t>
         </is>
       </c>
-      <c r="F13" t="inlineStr">
+      <c r="H13" t="inlineStr">
         <is>
           <t>4161</t>
         </is>
       </c>
-      <c r="G13" t="inlineStr">
+      <c r="I13" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="H13" t="inlineStr">
+      <c r="J13" t="inlineStr">
         <is>
           <t>1828</t>
         </is>
       </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="b">
@@ -1043,45 +1173,55 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>False</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
           <t>Iba O'Este</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
+      <c r="F14" t="inlineStr">
         <is>
           <t>14.8919</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr">
+      <c r="G14" t="inlineStr">
         <is>
           <t>120.7635</t>
         </is>
       </c>
-      <c r="F14" t="inlineStr">
+      <c r="H14" t="inlineStr">
         <is>
           <t>14085</t>
         </is>
       </c>
-      <c r="G14" t="inlineStr">
+      <c r="I14" t="inlineStr">
         <is>
           <t>601</t>
         </is>
       </c>
-      <c r="H14" t="inlineStr">
+      <c r="J14" t="inlineStr">
         <is>
           <t>8095</t>
         </is>
       </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="J14" t="inlineStr"/>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="b">
@@ -1089,45 +1229,55 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>False</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
           <t>Longos</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
+      <c r="F15" t="inlineStr">
         <is>
           <t>14.8748</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr">
+      <c r="G15" t="inlineStr">
         <is>
           <t>120.7866</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr">
+      <c r="H15" t="inlineStr">
         <is>
           <t>4265</t>
         </is>
       </c>
-      <c r="G15" t="inlineStr">
+      <c r="I15" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="H15" t="inlineStr">
+      <c r="J15" t="inlineStr">
         <is>
           <t>2293</t>
         </is>
       </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="J15" t="inlineStr"/>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="b">
@@ -1135,45 +1285,55 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>False</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
           <t>Meysulao</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
+      <c r="F16" t="inlineStr">
         <is>
           <t>14.9078</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr">
+      <c r="G16" t="inlineStr">
         <is>
           <t>120.7397</t>
         </is>
       </c>
-      <c r="F16" t="inlineStr">
+      <c r="H16" t="inlineStr">
         <is>
           <t>4280</t>
         </is>
       </c>
-      <c r="G16" t="inlineStr">
+      <c r="I16" t="inlineStr">
         <is>
           <t>56</t>
         </is>
       </c>
-      <c r="H16" t="inlineStr">
+      <c r="J16" t="inlineStr">
         <is>
           <t>2687</t>
         </is>
       </c>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="J16" t="inlineStr"/>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="b">
@@ -1181,45 +1341,55 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>False</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
           <t>Meyto</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr">
+      <c r="F17" t="inlineStr">
         <is>
           <t>14.8831</t>
         </is>
       </c>
-      <c r="E17" t="inlineStr">
+      <c r="G17" t="inlineStr">
         <is>
           <t>120.7295</t>
         </is>
       </c>
-      <c r="F17" t="inlineStr">
+      <c r="H17" t="inlineStr">
         <is>
           <t>2925</t>
         </is>
       </c>
-      <c r="G17" t="inlineStr">
+      <c r="I17" t="inlineStr">
         <is>
           <t>6</t>
         </is>
       </c>
-      <c r="H17" t="inlineStr">
+      <c r="J17" t="inlineStr">
         <is>
           <t>1975</t>
         </is>
       </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="J17" t="inlineStr"/>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="b">
@@ -1227,45 +1397,55 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>False</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
           <t>Palimbang</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr">
+      <c r="F18" t="inlineStr">
         <is>
           <t>14.8994</t>
         </is>
       </c>
-      <c r="E18" t="inlineStr">
+      <c r="G18" t="inlineStr">
         <is>
           <t>120.7756</t>
         </is>
       </c>
-      <c r="F18" t="inlineStr">
+      <c r="H18" t="inlineStr">
         <is>
           <t>1684</t>
         </is>
       </c>
-      <c r="G18" t="inlineStr">
+      <c r="I18" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="H18" t="inlineStr">
+      <c r="J18" t="inlineStr">
         <is>
           <t>1424</t>
         </is>
       </c>
-      <c r="I18" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="J18" t="inlineStr"/>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="b">
@@ -1273,45 +1453,55 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>False</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
           <t>Panducot</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr">
+      <c r="F19" t="inlineStr">
         <is>
           <t>14.8761</t>
         </is>
       </c>
-      <c r="E19" t="inlineStr">
+      <c r="G19" t="inlineStr">
         <is>
           <t>120.738</t>
         </is>
       </c>
-      <c r="F19" t="inlineStr">
+      <c r="H19" t="inlineStr">
         <is>
           <t>1752</t>
         </is>
       </c>
-      <c r="G19" t="inlineStr">
+      <c r="I19" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="H19" t="inlineStr">
+      <c r="J19" t="inlineStr">
         <is>
           <t>1713</t>
         </is>
       </c>
-      <c r="I19" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="J19" t="inlineStr"/>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="b">
@@ -1319,45 +1509,55 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>False</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
           <t>Poblacion</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr">
+      <c r="F20" t="inlineStr">
         <is>
           <t>14.9157</t>
         </is>
       </c>
-      <c r="E20" t="inlineStr">
+      <c r="G20" t="inlineStr">
         <is>
           <t>120.7672</t>
         </is>
       </c>
-      <c r="F20" t="inlineStr">
+      <c r="H20" t="inlineStr">
         <is>
           <t>1785</t>
         </is>
       </c>
-      <c r="G20" t="inlineStr">
+      <c r="I20" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="H20" t="inlineStr">
+      <c r="J20" t="inlineStr">
         <is>
           <t>1294</t>
         </is>
       </c>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="J20" t="inlineStr"/>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="b">
@@ -1365,45 +1565,55 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>False</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
           <t>Pungo</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr">
+      <c r="F21" t="inlineStr">
         <is>
           <t>14.9023</t>
         </is>
       </c>
-      <c r="E21" t="inlineStr">
+      <c r="G21" t="inlineStr">
         <is>
           <t>120.7914</t>
         </is>
       </c>
-      <c r="F21" t="inlineStr">
+      <c r="H21" t="inlineStr">
         <is>
           <t>9528</t>
         </is>
       </c>
-      <c r="G21" t="inlineStr">
+      <c r="I21" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="H21" t="inlineStr">
+      <c r="J21" t="inlineStr">
         <is>
           <t>5486</t>
         </is>
       </c>
-      <c r="I21" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="J21" t="inlineStr"/>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="b">
@@ -1411,45 +1621,55 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>False</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
           <t>San Jose</t>
         </is>
       </c>
-      <c r="D22" t="inlineStr">
+      <c r="F22" t="inlineStr">
         <is>
           <t>14.8838</t>
         </is>
       </c>
-      <c r="E22" t="inlineStr">
+      <c r="G22" t="inlineStr">
         <is>
           <t>120.7395</t>
         </is>
       </c>
-      <c r="F22" t="inlineStr">
+      <c r="H22" t="inlineStr">
         <is>
           <t>5661</t>
         </is>
       </c>
-      <c r="G22" t="inlineStr">
+      <c r="I22" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="H22" t="inlineStr">
+      <c r="J22" t="inlineStr">
         <is>
           <t>3629</t>
         </is>
       </c>
-      <c r="I22" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="J22" t="inlineStr"/>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="b">
@@ -1457,45 +1677,55 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>False</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
           <t>San Marcos</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr">
+      <c r="F23" t="inlineStr">
         <is>
           <t>14.8976</t>
         </is>
       </c>
-      <c r="E23" t="inlineStr">
+      <c r="G23" t="inlineStr">
         <is>
           <t>120.7797</t>
         </is>
       </c>
-      <c r="F23" t="inlineStr">
+      <c r="H23" t="inlineStr">
         <is>
           <t>2671</t>
         </is>
       </c>
-      <c r="G23" t="inlineStr">
+      <c r="I23" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="H23" t="inlineStr">
+      <c r="J23" t="inlineStr">
         <is>
           <t>1471</t>
         </is>
       </c>
-      <c r="I23" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="J23" t="inlineStr"/>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="b">
@@ -1503,45 +1733,55 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>False</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
           <t>San Miguel</t>
         </is>
       </c>
-      <c r="D24" t="inlineStr">
+      <c r="F24" t="inlineStr">
         <is>
           <t>14.917</t>
         </is>
       </c>
-      <c r="E24" t="inlineStr">
+      <c r="G24" t="inlineStr">
         <is>
           <t>120.7427</t>
         </is>
       </c>
-      <c r="F24" t="inlineStr">
+      <c r="H24" t="inlineStr">
         <is>
           <t>6005</t>
         </is>
       </c>
-      <c r="G24" t="inlineStr">
+      <c r="I24" t="inlineStr">
         <is>
           <t>17</t>
         </is>
       </c>
-      <c r="H24" t="inlineStr">
+      <c r="J24" t="inlineStr">
         <is>
           <t>3287</t>
         </is>
       </c>
-      <c r="I24" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="J24" t="inlineStr"/>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="b">
@@ -1549,45 +1789,55 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>False</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
           <t>Santa Lucia</t>
         </is>
       </c>
-      <c r="D25" t="inlineStr">
+      <c r="F25" t="inlineStr">
         <is>
           <t>14.8982</t>
         </is>
       </c>
-      <c r="E25" t="inlineStr">
+      <c r="G25" t="inlineStr">
         <is>
           <t>120.736</t>
         </is>
       </c>
-      <c r="F25" t="inlineStr">
+      <c r="H25" t="inlineStr">
         <is>
           <t>2460</t>
         </is>
       </c>
-      <c r="G25" t="inlineStr">
+      <c r="I25" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="H25" t="inlineStr">
+      <c r="J25" t="inlineStr">
         <is>
           <t>1483</t>
         </is>
       </c>
-      <c r="I25" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="J25" t="inlineStr"/>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="b">
@@ -1595,45 +1845,55 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>False</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
           <t>Santo Niño</t>
         </is>
       </c>
-      <c r="D26" t="inlineStr">
+      <c r="F26" t="inlineStr">
         <is>
           <t>14.9047</t>
         </is>
       </c>
-      <c r="E26" t="inlineStr">
+      <c r="G26" t="inlineStr">
         <is>
           <t>120.7792</t>
         </is>
       </c>
-      <c r="F26" t="inlineStr">
+      <c r="H26" t="inlineStr">
         <is>
           <t>2544</t>
         </is>
       </c>
-      <c r="G26" t="inlineStr">
+      <c r="I26" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="H26" t="inlineStr">
+      <c r="J26" t="inlineStr">
         <is>
           <t>1392</t>
         </is>
       </c>
-      <c r="I26" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="J26" t="inlineStr"/>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="b">
@@ -1641,45 +1901,55 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>False</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
           <t>Sapang Bayan</t>
         </is>
       </c>
-      <c r="D27" t="inlineStr">
+      <c r="F27" t="inlineStr">
         <is>
           <t>14.9196</t>
         </is>
       </c>
-      <c r="E27" t="inlineStr">
+      <c r="G27" t="inlineStr">
         <is>
           <t>120.7739</t>
         </is>
       </c>
-      <c r="F27" t="inlineStr">
+      <c r="H27" t="inlineStr">
         <is>
           <t>3140</t>
         </is>
       </c>
-      <c r="G27" t="inlineStr">
+      <c r="I27" t="inlineStr">
         <is>
           <t>65</t>
         </is>
       </c>
-      <c r="H27" t="inlineStr">
+      <c r="J27" t="inlineStr">
         <is>
           <t>1775</t>
         </is>
       </c>
-      <c r="I27" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="J27" t="inlineStr"/>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="b">
@@ -1687,133 +1957,163 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>False</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
           <t>Sergio Bayan</t>
         </is>
       </c>
-      <c r="D28" t="inlineStr">
+      <c r="F28" t="inlineStr">
         <is>
           <t>14.894</t>
         </is>
       </c>
-      <c r="E28" t="inlineStr">
+      <c r="G28" t="inlineStr">
         <is>
           <t>120.7909</t>
         </is>
       </c>
-      <c r="F28" t="inlineStr">
+      <c r="H28" t="inlineStr">
         <is>
           <t>1727</t>
         </is>
       </c>
-      <c r="G28" t="inlineStr">
+      <c r="I28" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="H28" t="inlineStr">
+      <c r="J28" t="inlineStr">
         <is>
           <t>1258</t>
         </is>
       </c>
-      <c r="I28" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="J28" t="inlineStr"/>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="L28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>False</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
           <t>Sucol</t>
         </is>
       </c>
-      <c r="D29" t="inlineStr">
+      <c r="F29" t="inlineStr">
         <is>
           <t>14.9138</t>
         </is>
       </c>
-      <c r="E29" t="inlineStr">
+      <c r="G29" t="inlineStr">
         <is>
           <t>120.7701</t>
         </is>
       </c>
-      <c r="F29" t="inlineStr">
+      <c r="H29" t="inlineStr">
         <is>
           <t>1059</t>
         </is>
       </c>
-      <c r="G29" t="inlineStr">
+      <c r="I29" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="H29" t="inlineStr">
+      <c r="J29" t="inlineStr">
         <is>
           <t>963</t>
         </is>
       </c>
-      <c r="I29" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="J29" t="inlineStr"/>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="L29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="b">
         <v>0</v>
       </c>
-      <c r="B30" t="inlineStr"/>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
       <c r="C30" t="inlineStr">
         <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr"/>
+      <c r="E30" t="inlineStr">
+        <is>
           <t>testAdd</t>
         </is>
       </c>
-      <c r="D30" t="inlineStr">
+      <c r="F30" t="inlineStr">
         <is>
           <t>120.0</t>
         </is>
       </c>
-      <c r="E30" t="inlineStr">
+      <c r="G30" t="inlineStr">
         <is>
           <t>12.0</t>
         </is>
       </c>
-      <c r="F30" t="inlineStr">
+      <c r="H30" t="inlineStr">
         <is>
           <t>23</t>
         </is>
       </c>
-      <c r="G30" t="inlineStr">
+      <c r="I30" t="inlineStr">
         <is>
           <t>23</t>
         </is>
       </c>
-      <c r="H30" t="inlineStr">
+      <c r="J30" t="inlineStr">
         <is>
           <t>32</t>
         </is>
       </c>
-      <c r="I30" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="J30" t="inlineStr">
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="L30" t="inlineStr">
         <is>
           <t>32.0</t>
         </is>

</xml_diff>

<commit_message>
Updated dashboard, Community fixed; checkbox to swtch
</commit_message>
<xml_diff>
--- a/ProgramSrc/commData.xlsx
+++ b/ProgramSrc/commData.xlsx
@@ -477,7 +477,7 @@
     </row>
     <row r="2">
       <c r="A2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -513,7 +513,7 @@
     </row>
     <row r="3">
       <c r="A3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
updating maps and focusing
</commit_message>
<xml_diff>
--- a/ProgramSrc/commData.xlsx
+++ b/ProgramSrc/commData.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -477,27 +477,27 @@
     </row>
     <row r="2">
       <c r="A2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Abangan Norte</t>
+          <t>Balite</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>120.9342</v>
+        <v>14.8956</v>
       </c>
       <c r="D2" t="n">
-        <v>14.7661</v>
+        <v>120.7855</v>
       </c>
       <c r="E2" t="n">
-        <v>11417</v>
+        <v>5016</v>
       </c>
       <c r="F2" t="n">
-        <v>10080</v>
+        <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="H2" t="inlineStr"/>
     </row>
@@ -507,23 +507,23 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Abangan Sur</t>
+          <t>Balungao</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>120.9437</v>
+        <v>14.9143</v>
       </c>
       <c r="D3" t="n">
-        <v>14.7653</v>
+        <v>120.7622</v>
       </c>
       <c r="E3" t="n">
-        <v>10595</v>
+        <v>5720</v>
       </c>
       <c r="F3" t="n">
-        <v>9750</v>
+        <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="H3" t="inlineStr"/>
     </row>
@@ -533,23 +533,23 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Ibayo</t>
+          <t>Buguion</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>120.9533</v>
+        <v>14.894</v>
       </c>
       <c r="D4" t="n">
-        <v>14.7535</v>
+        <v>120.7985</v>
       </c>
       <c r="E4" t="n">
-        <v>8310</v>
+        <v>3841</v>
       </c>
       <c r="F4" t="n">
-        <v>5000</v>
+        <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="H4" t="inlineStr"/>
     </row>
@@ -559,23 +559,23 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Lambakin</t>
+          <t>Bulusan</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>120.9785</v>
+        <v>14.9076</v>
       </c>
       <c r="D5" t="n">
-        <v>14.7738</v>
+        <v>120.7455</v>
       </c>
       <c r="E5" t="n">
-        <v>48184</v>
+        <v>2603</v>
       </c>
       <c r="F5" t="n">
-        <v>30000</v>
+        <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="H5" t="inlineStr"/>
     </row>
@@ -585,29 +585,25 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Lias</t>
+          <t>Calizon</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>120.9623</v>
+        <v>14.9125</v>
       </c>
       <c r="D6" t="n">
-        <v>14.7603</v>
+        <v>120.753</v>
       </c>
       <c r="E6" t="n">
-        <v>15256</v>
+        <v>2221</v>
       </c>
       <c r="F6" t="n">
-        <v>1545</v>
+        <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>2000</v>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>hmmm yes</t>
-        </is>
-      </c>
+        <v>1000</v>
+      </c>
+      <c r="H6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="b">
@@ -615,23 +611,23 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Loma de Gato</t>
+          <t>Caniogan</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>121.0077</v>
+        <v>14.9054</v>
       </c>
       <c r="D7" t="n">
-        <v>14.7911</v>
+        <v>120.7733</v>
       </c>
       <c r="E7" t="n">
-        <v>71258</v>
+        <v>4510</v>
       </c>
       <c r="F7" t="n">
-        <v>5000</v>
+        <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="H7" t="inlineStr"/>
     </row>
@@ -641,23 +637,23 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Nagbalon</t>
+          <t>Corazon</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>120.941</v>
+        <v>14.9128</v>
       </c>
       <c r="D8" t="n">
-        <v>14.7465</v>
+        <v>120.7686</v>
       </c>
       <c r="E8" t="n">
-        <v>3518</v>
+        <v>2175</v>
       </c>
       <c r="F8" t="n">
-        <v>4925</v>
+        <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="H8" t="inlineStr"/>
     </row>
@@ -667,23 +663,23 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Patubig</t>
+          <t>Frances</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>120.9595</v>
+        <v>14.9153</v>
       </c>
       <c r="D9" t="n">
-        <v>14.7774</v>
+        <v>120.7532</v>
       </c>
       <c r="E9" t="n">
-        <v>8419</v>
+        <v>6129</v>
       </c>
       <c r="F9" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="G9" t="n">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="H9" t="inlineStr"/>
     </row>
@@ -693,23 +689,23 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Poblacion I</t>
+          <t>Gatbuca</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>120.9488</v>
+        <v>14.9218</v>
       </c>
       <c r="D10" t="n">
-        <v>14.7559</v>
+        <v>120.7685</v>
       </c>
       <c r="E10" t="n">
-        <v>1419</v>
+        <v>6384</v>
       </c>
       <c r="F10" t="n">
-        <v>3000</v>
+        <v>115</v>
       </c>
       <c r="G10" t="n">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="H10" t="inlineStr"/>
     </row>
@@ -719,23 +715,23 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Poblacion II</t>
+          <t>Gugo</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>120.9464</v>
+        <v>14.9014</v>
       </c>
       <c r="D11" t="n">
-        <v>14.7599</v>
+        <v>120.7548</v>
       </c>
       <c r="E11" t="n">
-        <v>4968</v>
+        <v>1960</v>
       </c>
       <c r="F11" t="n">
-        <v>10000</v>
+        <v>57</v>
       </c>
       <c r="G11" t="n">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="H11" t="inlineStr"/>
     </row>
@@ -745,23 +741,23 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Prenza I</t>
+          <t>Iba Este</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>120.9849</v>
+        <v>14.8899</v>
       </c>
       <c r="D12" t="n">
-        <v>14.7833</v>
+        <v>120.7673</v>
       </c>
       <c r="E12" t="n">
-        <v>9019</v>
+        <v>4161</v>
       </c>
       <c r="F12" t="n">
-        <v>350</v>
+        <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="H12" t="inlineStr"/>
     </row>
@@ -771,23 +767,23 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Prenza II</t>
+          <t>Iba O'Este</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>120.9868</v>
+        <v>14.8919</v>
       </c>
       <c r="D13" t="n">
-        <v>14.7813</v>
+        <v>120.7635</v>
       </c>
       <c r="E13" t="n">
-        <v>13784</v>
+        <v>14085</v>
       </c>
       <c r="F13" t="n">
-        <v>3050</v>
+        <v>601</v>
       </c>
       <c r="G13" t="n">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="H13" t="inlineStr"/>
     </row>
@@ -797,23 +793,23 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Santa Rosa I</t>
+          <t>Meysulao</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>120.9746</v>
+        <v>14.9078</v>
       </c>
       <c r="D14" t="n">
-        <v>14.7789</v>
+        <v>120.7397</v>
       </c>
       <c r="E14" t="n">
-        <v>11260</v>
+        <v>4280</v>
       </c>
       <c r="F14" t="n">
-        <v>4995</v>
+        <v>56</v>
       </c>
       <c r="G14" t="n">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="H14" t="inlineStr"/>
     </row>
@@ -823,23 +819,23 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Santa Rosa II</t>
+          <t>Meyto</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>120.9686</v>
+        <v>14.8831</v>
       </c>
       <c r="D15" t="n">
-        <v>14.784</v>
+        <v>120.7295</v>
       </c>
       <c r="E15" t="n">
-        <v>13378</v>
+        <v>2925</v>
       </c>
       <c r="F15" t="n">
-        <v>4500</v>
+        <v>6</v>
       </c>
       <c r="G15" t="n">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="H15" t="inlineStr"/>
     </row>
@@ -849,23 +845,23 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Saog</t>
+          <t>Palimbang</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>120.9556</v>
+        <v>14.8994</v>
       </c>
       <c r="D16" t="n">
-        <v>14.7642</v>
+        <v>120.7756</v>
       </c>
       <c r="E16" t="n">
-        <v>15612</v>
+        <v>1684</v>
       </c>
       <c r="F16" t="n">
-        <v>15000</v>
+        <v>0</v>
       </c>
       <c r="G16" t="n">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="H16" t="inlineStr"/>
     </row>
@@ -875,55 +871,51 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Tabing Ilog</t>
+          <t>Panducot</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>120.9488</v>
+        <v>14.8761</v>
       </c>
       <c r="D17" t="n">
-        <v>14.7649</v>
+        <v>120.738</v>
       </c>
       <c r="E17" t="n">
-        <v>8056</v>
+        <v>1752</v>
       </c>
       <c r="F17" t="n">
-        <v>5500</v>
+        <v>0</v>
       </c>
       <c r="G17" t="n">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="H17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>we2</t>
+          <t>Pio Cruzcosa</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>3</v>
+        <v>14.8881</v>
       </c>
       <c r="D18" t="n">
-        <v>33</v>
+        <v>120.7855</v>
       </c>
       <c r="E18" t="n">
-        <v>3</v>
+        <v>4663</v>
       </c>
       <c r="F18" t="n">
-        <v>3</v>
+        <v>92</v>
       </c>
       <c r="G18" t="n">
-        <v>3</v>
-      </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>w</t>
-        </is>
-      </c>
+        <v>1000</v>
+      </c>
+      <c r="H18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="b">
@@ -931,35 +923,259 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>22</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>32</t>
-        </is>
+          <t>Poblacion</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>14.9157</v>
+      </c>
+      <c r="D19" t="n">
+        <v>120.7672</v>
+      </c>
+      <c r="E19" t="n">
+        <v>1785</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0</v>
+      </c>
+      <c r="G19" t="n">
+        <v>1000</v>
       </c>
       <c r="H19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="b">
+        <v>1</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Pungo</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>14.9023</v>
+      </c>
+      <c r="D20" t="n">
+        <v>120.7914</v>
+      </c>
+      <c r="E20" t="n">
+        <v>9528</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0</v>
+      </c>
+      <c r="G20" t="n">
+        <v>1000</v>
+      </c>
+      <c r="H20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="b">
+        <v>1</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>San Jose</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>14.8838</v>
+      </c>
+      <c r="D21" t="n">
+        <v>120.7395</v>
+      </c>
+      <c r="E21" t="n">
+        <v>5661</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0</v>
+      </c>
+      <c r="G21" t="n">
+        <v>1000</v>
+      </c>
+      <c r="H21" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="b">
+        <v>1</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>San Marcos</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>14.8976</v>
+      </c>
+      <c r="D22" t="n">
+        <v>120.7797</v>
+      </c>
+      <c r="E22" t="n">
+        <v>2671</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0</v>
+      </c>
+      <c r="G22" t="n">
+        <v>1000</v>
+      </c>
+      <c r="H22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="b">
+        <v>1</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>San Miguel</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>14.917</v>
+      </c>
+      <c r="D23" t="n">
+        <v>120.7427</v>
+      </c>
+      <c r="E23" t="n">
+        <v>6005</v>
+      </c>
+      <c r="F23" t="n">
+        <v>17</v>
+      </c>
+      <c r="G23" t="n">
+        <v>1000</v>
+      </c>
+      <c r="H23" t="inlineStr"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="b">
+        <v>1</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Santa Lucia</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>14.8982</v>
+      </c>
+      <c r="D24" t="n">
+        <v>120.736</v>
+      </c>
+      <c r="E24" t="n">
+        <v>2460</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0</v>
+      </c>
+      <c r="G24" t="n">
+        <v>1000</v>
+      </c>
+      <c r="H24" t="inlineStr"/>
+    </row>
+    <row r="25">
+      <c r="A25" t="b">
+        <v>1</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Santo Niño</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>14.9047</v>
+      </c>
+      <c r="D25" t="n">
+        <v>120.7792</v>
+      </c>
+      <c r="E25" t="n">
+        <v>2544</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0</v>
+      </c>
+      <c r="G25" t="n">
+        <v>1000</v>
+      </c>
+      <c r="H25" t="inlineStr"/>
+    </row>
+    <row r="26">
+      <c r="A26" t="b">
+        <v>1</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Sapang Bayan</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>14.9196</v>
+      </c>
+      <c r="D26" t="n">
+        <v>120.7739</v>
+      </c>
+      <c r="E26" t="n">
+        <v>3140</v>
+      </c>
+      <c r="F26" t="n">
+        <v>65</v>
+      </c>
+      <c r="G26" t="n">
+        <v>1000</v>
+      </c>
+      <c r="H26" t="inlineStr"/>
+    </row>
+    <row r="27">
+      <c r="A27" t="b">
+        <v>1</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Sergio Bayan</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>14.894</v>
+      </c>
+      <c r="D27" t="n">
+        <v>120.7909</v>
+      </c>
+      <c r="E27" t="n">
+        <v>1727</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0</v>
+      </c>
+      <c r="G27" t="n">
+        <v>1000</v>
+      </c>
+      <c r="H27" t="inlineStr"/>
+    </row>
+    <row r="28">
+      <c r="A28" t="b">
+        <v>1</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Sucol</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>14.9138</v>
+      </c>
+      <c r="D28" t="n">
+        <v>120.7701</v>
+      </c>
+      <c r="E28" t="n">
+        <v>1059</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0</v>
+      </c>
+      <c r="G28" t="n">
+        <v>1000</v>
+      </c>
+      <c r="H28" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
working filtering and active lightgray marker
</commit_message>
<xml_diff>
--- a/ProgramSrc/commData.xlsx
+++ b/ProgramSrc/commData.xlsx
@@ -484,254 +484,354 @@
           <t>Balite</t>
         </is>
       </c>
-      <c r="C2" t="n">
-        <v>14.8956</v>
-      </c>
-      <c r="D2" t="n">
-        <v>120.7855</v>
-      </c>
-      <c r="E2" t="n">
-        <v>5016</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G2" t="n">
-        <v>1000</v>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>14.8956</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>120.7855</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>5016</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
       </c>
       <c r="H2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
           <t>Balungao</t>
         </is>
       </c>
-      <c r="C3" t="n">
-        <v>14.9143</v>
-      </c>
-      <c r="D3" t="n">
-        <v>120.7622</v>
-      </c>
-      <c r="E3" t="n">
-        <v>5720</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G3" t="n">
-        <v>1000</v>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>14.9143</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>120.7622</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>5720</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
       </c>
       <c r="H3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
           <t>Buguion</t>
         </is>
       </c>
-      <c r="C4" t="n">
-        <v>14.894</v>
-      </c>
-      <c r="D4" t="n">
-        <v>120.7985</v>
-      </c>
-      <c r="E4" t="n">
-        <v>3841</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" t="n">
-        <v>1000</v>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>14.894</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>120.7985</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>3841</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
       </c>
       <c r="H4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
           <t>Bulusan</t>
         </is>
       </c>
-      <c r="C5" t="n">
-        <v>14.9076</v>
-      </c>
-      <c r="D5" t="n">
-        <v>120.7455</v>
-      </c>
-      <c r="E5" t="n">
-        <v>2603</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G5" t="n">
-        <v>1000</v>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>14.9076</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>120.7455</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>2603</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
       </c>
       <c r="H5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
           <t>Calizon</t>
         </is>
       </c>
-      <c r="C6" t="n">
-        <v>14.9125</v>
-      </c>
-      <c r="D6" t="n">
-        <v>120.753</v>
-      </c>
-      <c r="E6" t="n">
-        <v>2221</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G6" t="n">
-        <v>1000</v>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>14.9125</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>120.753</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>2221</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
       </c>
       <c r="H6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
           <t>Caniogan</t>
         </is>
       </c>
-      <c r="C7" t="n">
-        <v>14.9054</v>
-      </c>
-      <c r="D7" t="n">
-        <v>120.7733</v>
-      </c>
-      <c r="E7" t="n">
-        <v>4510</v>
-      </c>
-      <c r="F7" t="n">
-        <v>0</v>
-      </c>
-      <c r="G7" t="n">
-        <v>1000</v>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>14.9054</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>120.7733</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>4510</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
       </c>
       <c r="H7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
           <t>Corazon</t>
         </is>
       </c>
-      <c r="C8" t="n">
-        <v>14.9128</v>
-      </c>
-      <c r="D8" t="n">
-        <v>120.7686</v>
-      </c>
-      <c r="E8" t="n">
-        <v>2175</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0</v>
-      </c>
-      <c r="G8" t="n">
-        <v>1000</v>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>14.9128</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>120.7686</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>2175</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
       </c>
       <c r="H8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
           <t>Frances</t>
         </is>
       </c>
-      <c r="C9" t="n">
-        <v>14.9153</v>
-      </c>
-      <c r="D9" t="n">
-        <v>120.7532</v>
-      </c>
-      <c r="E9" t="n">
-        <v>6129</v>
-      </c>
-      <c r="F9" t="n">
-        <v>6</v>
-      </c>
-      <c r="G9" t="n">
-        <v>1000</v>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>14.9153</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>120.7532</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>6129</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
       </c>
       <c r="H9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
           <t>Gatbuca</t>
         </is>
       </c>
-      <c r="C10" t="n">
-        <v>14.9218</v>
-      </c>
-      <c r="D10" t="n">
-        <v>120.7685</v>
-      </c>
-      <c r="E10" t="n">
-        <v>6384</v>
-      </c>
-      <c r="F10" t="n">
-        <v>115</v>
-      </c>
-      <c r="G10" t="n">
-        <v>1000</v>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>14.9218</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>120.7685</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>6384</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>115</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
       </c>
       <c r="H10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
           <t>Gugo</t>
         </is>
       </c>
-      <c r="C11" t="n">
-        <v>14.9014</v>
-      </c>
-      <c r="D11" t="n">
-        <v>120.7548</v>
-      </c>
-      <c r="E11" t="n">
-        <v>1960</v>
-      </c>
-      <c r="F11" t="n">
-        <v>57</v>
-      </c>
-      <c r="G11" t="n">
-        <v>1000</v>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>14.9014</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>120.7548</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>1960</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>57</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
       </c>
       <c r="H11" t="inlineStr"/>
     </row>
@@ -744,20 +844,30 @@
           <t>Iba Este</t>
         </is>
       </c>
-      <c r="C12" t="n">
-        <v>14.8899</v>
-      </c>
-      <c r="D12" t="n">
-        <v>120.7673</v>
-      </c>
-      <c r="E12" t="n">
-        <v>4161</v>
-      </c>
-      <c r="F12" t="n">
-        <v>0</v>
-      </c>
-      <c r="G12" t="n">
-        <v>1000</v>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>14.8899</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>120.7673</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>4161</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
       </c>
       <c r="H12" t="inlineStr"/>
     </row>
@@ -770,20 +880,30 @@
           <t>Iba O'Este</t>
         </is>
       </c>
-      <c r="C13" t="n">
-        <v>14.8919</v>
-      </c>
-      <c r="D13" t="n">
-        <v>120.7635</v>
-      </c>
-      <c r="E13" t="n">
-        <v>14085</v>
-      </c>
-      <c r="F13" t="n">
-        <v>601</v>
-      </c>
-      <c r="G13" t="n">
-        <v>1000</v>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>14.8919</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>120.7635</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>14085</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>601</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
       </c>
       <c r="H13" t="inlineStr"/>
     </row>
@@ -796,20 +916,30 @@
           <t>Meysulao</t>
         </is>
       </c>
-      <c r="C14" t="n">
-        <v>14.9078</v>
-      </c>
-      <c r="D14" t="n">
-        <v>120.7397</v>
-      </c>
-      <c r="E14" t="n">
-        <v>4280</v>
-      </c>
-      <c r="F14" t="n">
-        <v>56</v>
-      </c>
-      <c r="G14" t="n">
-        <v>1000</v>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>14.9078</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>120.7397</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>4280</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>56</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
       </c>
       <c r="H14" t="inlineStr"/>
     </row>
@@ -822,20 +952,30 @@
           <t>Meyto</t>
         </is>
       </c>
-      <c r="C15" t="n">
-        <v>14.8831</v>
-      </c>
-      <c r="D15" t="n">
-        <v>120.7295</v>
-      </c>
-      <c r="E15" t="n">
-        <v>2925</v>
-      </c>
-      <c r="F15" t="n">
-        <v>6</v>
-      </c>
-      <c r="G15" t="n">
-        <v>1000</v>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>14.8831</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>120.7295</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>2925</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
       </c>
       <c r="H15" t="inlineStr"/>
     </row>
@@ -848,20 +988,30 @@
           <t>Palimbang</t>
         </is>
       </c>
-      <c r="C16" t="n">
-        <v>14.8994</v>
-      </c>
-      <c r="D16" t="n">
-        <v>120.7756</v>
-      </c>
-      <c r="E16" t="n">
-        <v>1684</v>
-      </c>
-      <c r="F16" t="n">
-        <v>0</v>
-      </c>
-      <c r="G16" t="n">
-        <v>1000</v>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>14.8994</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>120.7756</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>1684</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
       </c>
       <c r="H16" t="inlineStr"/>
     </row>
@@ -874,20 +1024,30 @@
           <t>Panducot</t>
         </is>
       </c>
-      <c r="C17" t="n">
-        <v>14.8761</v>
-      </c>
-      <c r="D17" t="n">
-        <v>120.738</v>
-      </c>
-      <c r="E17" t="n">
-        <v>1752</v>
-      </c>
-      <c r="F17" t="n">
-        <v>0</v>
-      </c>
-      <c r="G17" t="n">
-        <v>1000</v>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>14.8761</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>120.738</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>1752</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
       </c>
       <c r="H17" t="inlineStr"/>
     </row>
@@ -900,20 +1060,30 @@
           <t>Pio Cruzcosa</t>
         </is>
       </c>
-      <c r="C18" t="n">
-        <v>14.8881</v>
-      </c>
-      <c r="D18" t="n">
-        <v>120.7855</v>
-      </c>
-      <c r="E18" t="n">
-        <v>4663</v>
-      </c>
-      <c r="F18" t="n">
-        <v>92</v>
-      </c>
-      <c r="G18" t="n">
-        <v>1000</v>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>14.8881</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>120.7855</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>4663</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>92</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
       </c>
       <c r="H18" t="inlineStr"/>
     </row>
@@ -926,20 +1096,30 @@
           <t>Poblacion</t>
         </is>
       </c>
-      <c r="C19" t="n">
-        <v>14.9157</v>
-      </c>
-      <c r="D19" t="n">
-        <v>120.7672</v>
-      </c>
-      <c r="E19" t="n">
-        <v>1785</v>
-      </c>
-      <c r="F19" t="n">
-        <v>0</v>
-      </c>
-      <c r="G19" t="n">
-        <v>1000</v>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>14.9157</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>120.7672</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>1785</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
       </c>
       <c r="H19" t="inlineStr"/>
     </row>
@@ -952,46 +1132,66 @@
           <t>Pungo</t>
         </is>
       </c>
-      <c r="C20" t="n">
-        <v>14.9023</v>
-      </c>
-      <c r="D20" t="n">
-        <v>120.7914</v>
-      </c>
-      <c r="E20" t="n">
-        <v>9528</v>
-      </c>
-      <c r="F20" t="n">
-        <v>0</v>
-      </c>
-      <c r="G20" t="n">
-        <v>1000</v>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>14.9023</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>120.7914</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>9528</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
       </c>
       <c r="H20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
           <t>San Jose</t>
         </is>
       </c>
-      <c r="C21" t="n">
-        <v>14.8838</v>
-      </c>
-      <c r="D21" t="n">
-        <v>120.7395</v>
-      </c>
-      <c r="E21" t="n">
-        <v>5661</v>
-      </c>
-      <c r="F21" t="n">
-        <v>0</v>
-      </c>
-      <c r="G21" t="n">
-        <v>1000</v>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>14.8838</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>120.7395</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>5661</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
       </c>
       <c r="H21" t="inlineStr"/>
     </row>
@@ -1004,72 +1204,102 @@
           <t>San Marcos</t>
         </is>
       </c>
-      <c r="C22" t="n">
-        <v>14.8976</v>
-      </c>
-      <c r="D22" t="n">
-        <v>120.7797</v>
-      </c>
-      <c r="E22" t="n">
-        <v>2671</v>
-      </c>
-      <c r="F22" t="n">
-        <v>0</v>
-      </c>
-      <c r="G22" t="n">
-        <v>1000</v>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>14.8976</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>120.7797</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>2671</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
       </c>
       <c r="H22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
           <t>San Miguel</t>
         </is>
       </c>
-      <c r="C23" t="n">
-        <v>14.917</v>
-      </c>
-      <c r="D23" t="n">
-        <v>120.7427</v>
-      </c>
-      <c r="E23" t="n">
-        <v>6005</v>
-      </c>
-      <c r="F23" t="n">
-        <v>17</v>
-      </c>
-      <c r="G23" t="n">
-        <v>1000</v>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>14.917</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>120.7427</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>6005</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
       </c>
       <c r="H23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
           <t>Santa Lucia</t>
         </is>
       </c>
-      <c r="C24" t="n">
-        <v>14.8982</v>
-      </c>
-      <c r="D24" t="n">
-        <v>120.736</v>
-      </c>
-      <c r="E24" t="n">
-        <v>2460</v>
-      </c>
-      <c r="F24" t="n">
-        <v>0</v>
-      </c>
-      <c r="G24" t="n">
-        <v>1000</v>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>14.8982</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>120.736</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>2460</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
       </c>
       <c r="H24" t="inlineStr"/>
     </row>
@@ -1082,20 +1312,30 @@
           <t>Santo Niño</t>
         </is>
       </c>
-      <c r="C25" t="n">
-        <v>14.9047</v>
-      </c>
-      <c r="D25" t="n">
-        <v>120.7792</v>
-      </c>
-      <c r="E25" t="n">
-        <v>2544</v>
-      </c>
-      <c r="F25" t="n">
-        <v>0</v>
-      </c>
-      <c r="G25" t="n">
-        <v>1000</v>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>14.9047</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>120.7792</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>2544</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
       </c>
       <c r="H25" t="inlineStr"/>
     </row>
@@ -1108,20 +1348,30 @@
           <t>Sapang Bayan</t>
         </is>
       </c>
-      <c r="C26" t="n">
-        <v>14.9196</v>
-      </c>
-      <c r="D26" t="n">
-        <v>120.7739</v>
-      </c>
-      <c r="E26" t="n">
-        <v>3140</v>
-      </c>
-      <c r="F26" t="n">
-        <v>65</v>
-      </c>
-      <c r="G26" t="n">
-        <v>1000</v>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>14.9196</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>120.7739</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>3140</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
       </c>
       <c r="H26" t="inlineStr"/>
     </row>
@@ -1134,20 +1384,30 @@
           <t>Sergio Bayan</t>
         </is>
       </c>
-      <c r="C27" t="n">
-        <v>14.894</v>
-      </c>
-      <c r="D27" t="n">
-        <v>120.7909</v>
-      </c>
-      <c r="E27" t="n">
-        <v>1727</v>
-      </c>
-      <c r="F27" t="n">
-        <v>0</v>
-      </c>
-      <c r="G27" t="n">
-        <v>1000</v>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>14.894</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>120.7909</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>1727</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
       </c>
       <c r="H27" t="inlineStr"/>
     </row>
@@ -1160,20 +1420,30 @@
           <t>Sucol</t>
         </is>
       </c>
-      <c r="C28" t="n">
-        <v>14.9138</v>
-      </c>
-      <c r="D28" t="n">
-        <v>120.7701</v>
-      </c>
-      <c r="E28" t="n">
-        <v>1059</v>
-      </c>
-      <c r="F28" t="n">
-        <v>0</v>
-      </c>
-      <c r="G28" t="n">
-        <v>1000</v>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>14.9138</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>120.7701</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>1059</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
       </c>
       <c r="H28" t="inlineStr"/>
     </row>

</xml_diff>

<commit_message>
updating list on dashboard and solveSettings
</commit_message>
<xml_diff>
--- a/ProgramSrc/commData.xlsx
+++ b/ProgramSrc/commData.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H28"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -481,22 +481,22 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Balite</t>
+          <t>dicsa</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>14.8956</t>
+          <t>14.894</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>120.7855</t>
+          <t>120.7985</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>5016</t>
+          <t>3841</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -517,22 +517,22 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Balungao</t>
+          <t>Bulusan</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>14.9143</t>
+          <t>14.9076</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>120.7622</t>
+          <t>120.7455</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>5720</t>
+          <t>2603</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -553,22 +553,22 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Buguion</t>
+          <t>Calizon</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>14.894</t>
+          <t>14.9125</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>120.7985</t>
+          <t>120.753</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>3841</t>
+          <t>2221</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -589,22 +589,22 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Bulusan</t>
+          <t>Caniogan</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>14.9076</t>
+          <t>14.9054</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>120.7455</t>
+          <t>120.7733</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2603</t>
+          <t>4510</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -625,22 +625,22 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Calizon</t>
+          <t>Corazon</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>14.9125</t>
+          <t>14.9128</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>120.753</t>
+          <t>120.7686</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2221</t>
+          <t>2175</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -661,27 +661,27 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Caniogan</t>
+          <t>Frances</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>14.9054</t>
+          <t>14.9153</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>120.7733</t>
+          <t>120.7532</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>4510</t>
+          <t>6129</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>6</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -697,27 +697,27 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Corazon</t>
+          <t>Gatbuca</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>14.9128</t>
+          <t>14.9218</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>120.7686</t>
+          <t>120.7685</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2175</t>
+          <t>6384</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>115</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -733,27 +733,27 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Frances</t>
+          <t>Gugo</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>14.9153</t>
+          <t>14.9014</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>120.7532</t>
+          <t>120.7548</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>6129</t>
+          <t>1960</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>57</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -769,27 +769,27 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Gatbuca</t>
+          <t>Iba Este</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>14.9218</t>
+          <t>14.8899</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>120.7685</t>
+          <t>120.7673</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>6384</t>
+          <t>4161</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>115</t>
+          <t>0</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -805,27 +805,27 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Gugo</t>
+          <t>Iba O'Este</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>14.9014</t>
+          <t>14.8919</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>120.7548</t>
+          <t>120.7635</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1960</t>
+          <t>14085</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>57</t>
+          <t>601</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -837,31 +837,31 @@
     </row>
     <row r="12">
       <c r="A12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Iba Este</t>
+          <t>Meysulao</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>14.8899</t>
+          <t>14.9078</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>120.7673</t>
+          <t>120.7397</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>4161</t>
+          <t>4280</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>56</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -877,27 +877,27 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Iba O'Este</t>
+          <t>Meyto</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>14.8919</t>
+          <t>14.8831</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>120.7635</t>
+          <t>120.7295</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>14085</t>
+          <t>2925</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>601</t>
+          <t>6</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
@@ -913,27 +913,27 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Meysulao</t>
+          <t>Palimbang</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>14.9078</t>
+          <t>14.8994</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>120.7397</t>
+          <t>120.7756</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>4280</t>
+          <t>1684</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>56</t>
+          <t>0</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
@@ -949,27 +949,27 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Meyto</t>
+          <t>Panducot</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>14.8831</t>
+          <t>14.8761</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>120.7295</t>
+          <t>120.738</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>2925</t>
+          <t>1752</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>0</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
@@ -985,27 +985,27 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Palimbang</t>
+          <t>Pio Cruzcosa</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>14.8994</t>
+          <t>14.8881</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>120.7756</t>
+          <t>120.7855</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>1684</t>
+          <t>4663</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>92</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -1021,22 +1021,22 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Panducot</t>
+          <t>Poblacion</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>14.8761</t>
+          <t>14.9157</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>120.738</t>
+          <t>120.7672</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1752</t>
+          <t>1785</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1053,31 +1053,31 @@
     </row>
     <row r="18">
       <c r="A18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Pio Cruzcosa</t>
+          <t>Pungo</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>14.8881</t>
+          <t>14.9023</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>120.7855</t>
+          <t>120.7914</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>4663</t>
+          <t>9528</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>92</t>
+          <t>0</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
@@ -1089,26 +1089,26 @@
     </row>
     <row r="19">
       <c r="A19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Poblacion</t>
+          <t>San Jose</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>14.9157</t>
+          <t>14.8838</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>120.7672</t>
+          <t>120.7395</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>1785</t>
+          <t>5661</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1129,22 +1129,22 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Pungo</t>
+          <t>San Marcos</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>14.9023</t>
+          <t>14.8976</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>120.7914</t>
+          <t>120.7797</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>9528</t>
+          <t>2671</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1165,27 +1165,27 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>San Jose</t>
+          <t>San Miguel</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>14.8838</t>
+          <t>14.917</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>120.7395</t>
+          <t>120.7427</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>5661</t>
+          <t>6005</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>17</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
@@ -1197,26 +1197,26 @@
     </row>
     <row r="22">
       <c r="A22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>San Marcos</t>
+          <t>Santa Lucia</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>14.8976</t>
+          <t>14.8982</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>120.7797</t>
+          <t>120.736</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>2671</t>
+          <t>2460</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -1233,31 +1233,31 @@
     </row>
     <row r="23">
       <c r="A23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>San Miguel</t>
+          <t>Santo Niño</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>14.917</t>
+          <t>14.9047</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>120.7427</t>
+          <t>120.7792</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>6005</t>
+          <t>2544</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>0</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
@@ -1269,31 +1269,31 @@
     </row>
     <row r="24">
       <c r="A24" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Santa Lucia</t>
+          <t>Sapang Bayan</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>14.8982</t>
+          <t>14.9196</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>120.736</t>
+          <t>120.7739</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>2460</t>
+          <t>3140</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>65</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
@@ -1309,22 +1309,22 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Santo Niño</t>
+          <t>Sergio Bayan</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>14.9047</t>
+          <t>14.894</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>120.7792</t>
+          <t>120.7909</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>2544</t>
+          <t>1727</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -1345,27 +1345,27 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Sapang Bayan</t>
+          <t>Sucol</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>14.9196</t>
+          <t>14.9138</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>120.7739</t>
+          <t>120.7701</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>3140</t>
+          <t>1059</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>65</t>
+          <t>0</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
@@ -1374,78 +1374,6 @@
         </is>
       </c>
       <c r="H26" t="inlineStr"/>
-    </row>
-    <row r="27">
-      <c r="A27" t="b">
-        <v>1</v>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>Sergio Bayan</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>14.894</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>120.7909</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>1727</t>
-        </is>
-      </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="H27" t="inlineStr"/>
-    </row>
-    <row r="28">
-      <c r="A28" t="b">
-        <v>1</v>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>Sucol</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>14.9138</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>120.7701</t>
-        </is>
-      </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>1059</t>
-        </is>
-      </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="H28" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
not hanging, working cancel
</commit_message>
<xml_diff>
--- a/ProgramSrc/commData.xlsx
+++ b/ProgramSrc/commData.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -484,32 +484,52 @@
           <t>Pio Cruzcosa</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>14.8881</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>120.7855</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>4663</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>92</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
+      <c r="C2" t="n">
+        <v>14.8881</v>
+      </c>
+      <c r="D2" t="n">
+        <v>120.7855</v>
+      </c>
+      <c r="E2" t="n">
+        <v>4663</v>
+      </c>
+      <c r="F2" t="n">
+        <v>92</v>
+      </c>
+      <c r="G2" t="n">
+        <v>1000</v>
       </c>
       <c r="H2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="b">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>bry</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>14.9</v>
+      </c>
+      <c r="D3" t="n">
+        <v>120.78</v>
+      </c>
+      <c r="E3" t="n">
+        <v>3</v>
+      </c>
+      <c r="F3" t="n">
+        <v>3</v>
+      </c>
+      <c r="G3" t="n">
+        <v>2</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
working GA with filtered data
</commit_message>
<xml_diff>
--- a/ProgramSrc/commData.xlsx
+++ b/ProgramSrc/commData.xlsx
@@ -484,20 +484,30 @@
           <t>Pio Cruzcosa</t>
         </is>
       </c>
-      <c r="C2" t="n">
-        <v>14.8881</v>
-      </c>
-      <c r="D2" t="n">
-        <v>120.7855</v>
-      </c>
-      <c r="E2" t="n">
-        <v>4663</v>
-      </c>
-      <c r="F2" t="n">
-        <v>92</v>
-      </c>
-      <c r="G2" t="n">
-        <v>1000</v>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>14.8881</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>120.7855</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>4663</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>92</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
       </c>
       <c r="H2" t="inlineStr"/>
     </row>
@@ -510,20 +520,30 @@
           <t>bry</t>
         </is>
       </c>
-      <c r="C3" t="n">
-        <v>14.9</v>
-      </c>
-      <c r="D3" t="n">
-        <v>120.78</v>
-      </c>
-      <c r="E3" t="n">
-        <v>3</v>
-      </c>
-      <c r="F3" t="n">
-        <v>3</v>
-      </c>
-      <c r="G3" t="n">
-        <v>2</v>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>14.9</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>120.78</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
saving allocation results; added report ui
</commit_message>
<xml_diff>
--- a/ProgramSrc/commData.xlsx
+++ b/ProgramSrc/commData.xlsx
@@ -484,20 +484,30 @@
           <t>Balite</t>
         </is>
       </c>
-      <c r="C2" t="n">
-        <v>14.8956</v>
-      </c>
-      <c r="D2" t="n">
-        <v>120.7855</v>
-      </c>
-      <c r="E2" t="n">
-        <v>5016</v>
-      </c>
-      <c r="F2" t="n">
-        <v>45454544</v>
-      </c>
-      <c r="G2" t="n">
-        <v>1000</v>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>14.8956</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>120.7855</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>5016</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
       </c>
       <c r="H2" t="inlineStr"/>
     </row>
@@ -510,20 +520,30 @@
           <t>Balungao</t>
         </is>
       </c>
-      <c r="C3" t="n">
-        <v>14.9143</v>
-      </c>
-      <c r="D3" t="n">
-        <v>120.7622</v>
-      </c>
-      <c r="E3" t="n">
-        <v>5720</v>
-      </c>
-      <c r="F3" t="n">
-        <v>52000</v>
-      </c>
-      <c r="G3" t="n">
-        <v>1000</v>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>14.9143</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>120.7622</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>5720</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
       </c>
       <c r="H3" t="inlineStr"/>
     </row>
@@ -536,20 +556,30 @@
           <t>Buguion</t>
         </is>
       </c>
-      <c r="C4" t="n">
-        <v>14.894</v>
-      </c>
-      <c r="D4" t="n">
-        <v>120.7985</v>
-      </c>
-      <c r="E4" t="n">
-        <v>3841</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" t="n">
-        <v>1000</v>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>14.894</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>120.7985</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>3841</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
       </c>
       <c r="H4" t="inlineStr"/>
     </row>
@@ -562,20 +592,30 @@
           <t>Bulusan</t>
         </is>
       </c>
-      <c r="C5" t="n">
-        <v>14.9076</v>
-      </c>
-      <c r="D5" t="n">
-        <v>120.7455</v>
-      </c>
-      <c r="E5" t="n">
-        <v>2603</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G5" t="n">
-        <v>1000</v>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>14.9076</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>120.7455</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>2603</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
       </c>
       <c r="H5" t="inlineStr"/>
     </row>
@@ -588,20 +628,30 @@
           <t>Calizon</t>
         </is>
       </c>
-      <c r="C6" t="n">
-        <v>14.9125</v>
-      </c>
-      <c r="D6" t="n">
-        <v>120.753</v>
-      </c>
-      <c r="E6" t="n">
-        <v>2221</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G6" t="n">
-        <v>1000</v>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>14.9125</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>120.753</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>2221</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
       </c>
       <c r="H6" t="inlineStr"/>
     </row>
@@ -614,20 +664,30 @@
           <t>Calumpang</t>
         </is>
       </c>
-      <c r="C7" t="n">
-        <v>14.8845</v>
-      </c>
-      <c r="D7" t="n">
-        <v>120.7838</v>
-      </c>
-      <c r="E7" t="n">
-        <v>3517</v>
-      </c>
-      <c r="F7" t="n">
-        <v>0</v>
-      </c>
-      <c r="G7" t="n">
-        <v>1000</v>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>14.8845</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>120.7838</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>3517</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
       </c>
       <c r="H7" t="inlineStr"/>
     </row>
@@ -640,20 +700,30 @@
           <t>Caniogan</t>
         </is>
       </c>
-      <c r="C8" t="n">
-        <v>14.9054</v>
-      </c>
-      <c r="D8" t="n">
-        <v>120.7733</v>
-      </c>
-      <c r="E8" t="n">
-        <v>4510</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0</v>
-      </c>
-      <c r="G8" t="n">
-        <v>1000</v>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>14.9054</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>120.7733</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>4510</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
       </c>
       <c r="H8" t="inlineStr"/>
     </row>
@@ -666,20 +736,30 @@
           <t>Corazon</t>
         </is>
       </c>
-      <c r="C9" t="n">
-        <v>14.9128</v>
-      </c>
-      <c r="D9" t="n">
-        <v>120.7686</v>
-      </c>
-      <c r="E9" t="n">
-        <v>2175</v>
-      </c>
-      <c r="F9" t="n">
-        <v>0</v>
-      </c>
-      <c r="G9" t="n">
-        <v>1000</v>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>14.9128</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>120.7686</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>2175</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
       </c>
       <c r="H9" t="inlineStr"/>
     </row>
@@ -692,20 +772,30 @@
           <t>Frances</t>
         </is>
       </c>
-      <c r="C10" t="n">
-        <v>14.9153</v>
-      </c>
-      <c r="D10" t="n">
-        <v>120.7532</v>
-      </c>
-      <c r="E10" t="n">
-        <v>6129</v>
-      </c>
-      <c r="F10" t="n">
-        <v>6</v>
-      </c>
-      <c r="G10" t="n">
-        <v>1000</v>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>14.9153</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>120.7532</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>6129</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
       </c>
       <c r="H10" t="inlineStr"/>
     </row>
@@ -718,20 +808,30 @@
           <t>Gatbuca</t>
         </is>
       </c>
-      <c r="C11" t="n">
-        <v>14.9218</v>
-      </c>
-      <c r="D11" t="n">
-        <v>120.7685</v>
-      </c>
-      <c r="E11" t="n">
-        <v>6384</v>
-      </c>
-      <c r="F11" t="n">
-        <v>115</v>
-      </c>
-      <c r="G11" t="n">
-        <v>1000</v>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>14.9218</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>120.7685</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>6384</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>115</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
       </c>
       <c r="H11" t="inlineStr"/>
     </row>
@@ -744,20 +844,30 @@
           <t>Gugo</t>
         </is>
       </c>
-      <c r="C12" t="n">
-        <v>14.9014</v>
-      </c>
-      <c r="D12" t="n">
-        <v>120.7548</v>
-      </c>
-      <c r="E12" t="n">
-        <v>1960</v>
-      </c>
-      <c r="F12" t="n">
-        <v>57</v>
-      </c>
-      <c r="G12" t="n">
-        <v>1000</v>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>14.9014</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>120.7548</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>1960</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>57</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
       </c>
       <c r="H12" t="inlineStr"/>
     </row>
@@ -770,20 +880,30 @@
           <t>Iba Este</t>
         </is>
       </c>
-      <c r="C13" t="n">
-        <v>14.8899</v>
-      </c>
-      <c r="D13" t="n">
-        <v>120.7673</v>
-      </c>
-      <c r="E13" t="n">
-        <v>4161</v>
-      </c>
-      <c r="F13" t="n">
-        <v>0</v>
-      </c>
-      <c r="G13" t="n">
-        <v>1000</v>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>14.8899</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>120.7673</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>4161</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
       </c>
       <c r="H13" t="inlineStr"/>
     </row>
@@ -796,20 +916,30 @@
           <t>Iba O'Este</t>
         </is>
       </c>
-      <c r="C14" t="n">
-        <v>14.8919</v>
-      </c>
-      <c r="D14" t="n">
-        <v>120.7635</v>
-      </c>
-      <c r="E14" t="n">
-        <v>14085</v>
-      </c>
-      <c r="F14" t="n">
-        <v>601</v>
-      </c>
-      <c r="G14" t="n">
-        <v>1000</v>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>14.8919</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>120.7635</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>14085</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>601</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
       </c>
       <c r="H14" t="inlineStr"/>
     </row>
@@ -822,20 +952,30 @@
           <t>Longos</t>
         </is>
       </c>
-      <c r="C15" t="n">
-        <v>14.8748</v>
-      </c>
-      <c r="D15" t="n">
-        <v>120.7866</v>
-      </c>
-      <c r="E15" t="n">
-        <v>4265</v>
-      </c>
-      <c r="F15" t="n">
-        <v>0</v>
-      </c>
-      <c r="G15" t="n">
-        <v>1000</v>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>14.8748</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>120.7866</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>4265</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
       </c>
       <c r="H15" t="inlineStr"/>
     </row>
@@ -848,20 +988,30 @@
           <t>Meysulao</t>
         </is>
       </c>
-      <c r="C16" t="n">
-        <v>14.9078</v>
-      </c>
-      <c r="D16" t="n">
-        <v>120.7397</v>
-      </c>
-      <c r="E16" t="n">
-        <v>4280</v>
-      </c>
-      <c r="F16" t="n">
-        <v>56</v>
-      </c>
-      <c r="G16" t="n">
-        <v>1000</v>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>14.9078</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>120.7397</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>4280</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>56</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
       </c>
       <c r="H16" t="inlineStr"/>
     </row>
@@ -874,20 +1024,30 @@
           <t>Meyto</t>
         </is>
       </c>
-      <c r="C17" t="n">
-        <v>14.8831</v>
-      </c>
-      <c r="D17" t="n">
-        <v>120.7295</v>
-      </c>
-      <c r="E17" t="n">
-        <v>2925</v>
-      </c>
-      <c r="F17" t="n">
-        <v>6</v>
-      </c>
-      <c r="G17" t="n">
-        <v>1000</v>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>14.8831</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>120.7295</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>2925</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
       </c>
       <c r="H17" t="inlineStr"/>
     </row>
@@ -900,20 +1060,30 @@
           <t>Palimbang</t>
         </is>
       </c>
-      <c r="C18" t="n">
-        <v>14.8994</v>
-      </c>
-      <c r="D18" t="n">
-        <v>120.7756</v>
-      </c>
-      <c r="E18" t="n">
-        <v>1684</v>
-      </c>
-      <c r="F18" t="n">
-        <v>0</v>
-      </c>
-      <c r="G18" t="n">
-        <v>1000</v>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>14.8994</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>120.7756</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>1684</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
       </c>
       <c r="H18" t="inlineStr"/>
     </row>
@@ -926,20 +1096,30 @@
           <t>Panducot</t>
         </is>
       </c>
-      <c r="C19" t="n">
-        <v>14.8761</v>
-      </c>
-      <c r="D19" t="n">
-        <v>120.738</v>
-      </c>
-      <c r="E19" t="n">
-        <v>1752</v>
-      </c>
-      <c r="F19" t="n">
-        <v>0</v>
-      </c>
-      <c r="G19" t="n">
-        <v>1000</v>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>14.8761</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>120.738</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>1752</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
       </c>
       <c r="H19" t="inlineStr"/>
     </row>
@@ -952,20 +1132,30 @@
           <t>Pio Cruzcosa</t>
         </is>
       </c>
-      <c r="C20" t="n">
-        <v>14.8881</v>
-      </c>
-      <c r="D20" t="n">
-        <v>120.7855</v>
-      </c>
-      <c r="E20" t="n">
-        <v>4663</v>
-      </c>
-      <c r="F20" t="n">
-        <v>92</v>
-      </c>
-      <c r="G20" t="n">
-        <v>1000</v>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>14.8881</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>120.7855</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>4663</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>92</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
       </c>
       <c r="H20" t="inlineStr"/>
     </row>
@@ -978,20 +1168,30 @@
           <t>Poblacion</t>
         </is>
       </c>
-      <c r="C21" t="n">
-        <v>14.9157</v>
-      </c>
-      <c r="D21" t="n">
-        <v>120.7672</v>
-      </c>
-      <c r="E21" t="n">
-        <v>1785</v>
-      </c>
-      <c r="F21" t="n">
-        <v>0</v>
-      </c>
-      <c r="G21" t="n">
-        <v>1000</v>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>14.9157</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>120.7672</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>1785</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
       </c>
       <c r="H21" t="inlineStr"/>
     </row>
@@ -1004,20 +1204,30 @@
           <t>Pungo</t>
         </is>
       </c>
-      <c r="C22" t="n">
-        <v>14.9023</v>
-      </c>
-      <c r="D22" t="n">
-        <v>120.7914</v>
-      </c>
-      <c r="E22" t="n">
-        <v>9528</v>
-      </c>
-      <c r="F22" t="n">
-        <v>0</v>
-      </c>
-      <c r="G22" t="n">
-        <v>1000</v>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>14.9023</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>120.7914</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>9528</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
       </c>
       <c r="H22" t="inlineStr"/>
     </row>
@@ -1030,20 +1240,30 @@
           <t>San Jose</t>
         </is>
       </c>
-      <c r="C23" t="n">
-        <v>14.8838</v>
-      </c>
-      <c r="D23" t="n">
-        <v>120.7395</v>
-      </c>
-      <c r="E23" t="n">
-        <v>5661</v>
-      </c>
-      <c r="F23" t="n">
-        <v>0</v>
-      </c>
-      <c r="G23" t="n">
-        <v>1000</v>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>14.8838</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>120.7395</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>5661</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
       </c>
       <c r="H23" t="inlineStr"/>
     </row>
@@ -1056,20 +1276,30 @@
           <t>San Marcos</t>
         </is>
       </c>
-      <c r="C24" t="n">
-        <v>14.8976</v>
-      </c>
-      <c r="D24" t="n">
-        <v>120.7797</v>
-      </c>
-      <c r="E24" t="n">
-        <v>2671</v>
-      </c>
-      <c r="F24" t="n">
-        <v>0</v>
-      </c>
-      <c r="G24" t="n">
-        <v>1000</v>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>14.8976</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>120.7797</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>2671</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
       </c>
       <c r="H24" t="inlineStr"/>
     </row>
@@ -1082,20 +1312,30 @@
           <t>San Miguel</t>
         </is>
       </c>
-      <c r="C25" t="n">
-        <v>14.917</v>
-      </c>
-      <c r="D25" t="n">
-        <v>120.7427</v>
-      </c>
-      <c r="E25" t="n">
-        <v>6005</v>
-      </c>
-      <c r="F25" t="n">
-        <v>17</v>
-      </c>
-      <c r="G25" t="n">
-        <v>1000</v>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>14.917</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>120.7427</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>6005</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
       </c>
       <c r="H25" t="inlineStr"/>
     </row>
@@ -1108,20 +1348,30 @@
           <t>Santa Lucia</t>
         </is>
       </c>
-      <c r="C26" t="n">
-        <v>14.8982</v>
-      </c>
-      <c r="D26" t="n">
-        <v>120.736</v>
-      </c>
-      <c r="E26" t="n">
-        <v>2460</v>
-      </c>
-      <c r="F26" t="n">
-        <v>0</v>
-      </c>
-      <c r="G26" t="n">
-        <v>1000</v>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>14.8982</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>120.736</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>2460</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
       </c>
       <c r="H26" t="inlineStr"/>
     </row>
@@ -1134,20 +1384,30 @@
           <t>Santo Niño</t>
         </is>
       </c>
-      <c r="C27" t="n">
-        <v>14.9047</v>
-      </c>
-      <c r="D27" t="n">
-        <v>120.7792</v>
-      </c>
-      <c r="E27" t="n">
-        <v>2544</v>
-      </c>
-      <c r="F27" t="n">
-        <v>0</v>
-      </c>
-      <c r="G27" t="n">
-        <v>1000</v>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>14.9047</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>120.7792</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>2544</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
       </c>
       <c r="H27" t="inlineStr"/>
     </row>
@@ -1160,20 +1420,30 @@
           <t>Sapang Bayan</t>
         </is>
       </c>
-      <c r="C28" t="n">
-        <v>14.9196</v>
-      </c>
-      <c r="D28" t="n">
-        <v>120.7739</v>
-      </c>
-      <c r="E28" t="n">
-        <v>3140</v>
-      </c>
-      <c r="F28" t="n">
-        <v>65</v>
-      </c>
-      <c r="G28" t="n">
-        <v>1000</v>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>14.9196</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>120.7739</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>3140</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
       </c>
       <c r="H28" t="inlineStr"/>
     </row>
@@ -1186,20 +1456,30 @@
           <t>Sergio Bayan</t>
         </is>
       </c>
-      <c r="C29" t="n">
-        <v>14.894</v>
-      </c>
-      <c r="D29" t="n">
-        <v>120.7909</v>
-      </c>
-      <c r="E29" t="n">
-        <v>1727</v>
-      </c>
-      <c r="F29" t="n">
-        <v>0</v>
-      </c>
-      <c r="G29" t="n">
-        <v>1000</v>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>14.894</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>120.7909</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>1727</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
       </c>
       <c r="H29" t="inlineStr"/>
     </row>
@@ -1212,20 +1492,30 @@
           <t>Sucol</t>
         </is>
       </c>
-      <c r="C30" t="n">
-        <v>14.9138</v>
-      </c>
-      <c r="D30" t="n">
-        <v>120.7701</v>
-      </c>
-      <c r="E30" t="n">
-        <v>1059</v>
-      </c>
-      <c r="F30" t="n">
-        <v>0</v>
-      </c>
-      <c r="G30" t="n">
-        <v>1000</v>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>14.9138</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>120.7701</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>1059</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
       </c>
       <c r="H30" t="inlineStr"/>
     </row>

</xml_diff>